<commit_message>
Fix spreadsheet parsing errors
</commit_message>
<xml_diff>
--- a/spreadsheets/Anivia.xlsx
+++ b/spreadsheets/Anivia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunny\champs.gg\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A77833-A319-4328-BC73-017FD9EE35FF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3EC9AB0-A7A2-4F1D-9F78-98F2B549AF39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{B545EDFA-6363-4C2A-9C9C-217A6E7A6E38}"/>
+    <workbookView xWindow="3060" yWindow="1050" windowWidth="16875" windowHeight="10522" xr2:uid="{B545EDFA-6363-4C2A-9C9C-217A6E7A6E38}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="132">
   <si>
     <t>id</t>
   </si>
@@ -59,9 +59,6 @@
   </si>
   <si>
     <t>If you aren't sure for portrait, just send me the picture you want on discord (usephysics#0001)</t>
-  </si>
-  <si>
-    <t>Once you have filled this out, please change sheets at the bottom.</t>
   </si>
   <si>
     <t>Champion</t>
@@ -505,13 +502,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>10309</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -555,13 +552,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>9526</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>169743</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>245812</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -901,150 +898,145 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1FF1A3E-B1DC-4DEF-A1FF-05C516225EE7}">
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="160.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="160.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1328125" customWidth="1"/>
+    <col min="4" max="4" width="9.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" t="s">
         <v>131</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B8" t="s">
-        <v>81</v>
-      </c>
-      <c r="C8" s="1" t="s">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" t="s">
-        <v>126</v>
-      </c>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="C13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O13" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="B11" t="s">
-        <v>132</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C12" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1052,7 +1044,7 @@
     <hyperlink ref="B4" r:id="rId1" xr:uid="{5BE9A3BD-50A3-4498-9281-460AF4B05C45}"/>
     <hyperlink ref="B5" r:id="rId2" xr:uid="{EF053C2E-238E-43C8-AF8E-41ACE05E4B59}"/>
     <hyperlink ref="B6" r:id="rId3" xr:uid="{EAAE58AD-F9EF-4280-B06D-9BCA4BAFF1B6}"/>
-    <hyperlink ref="B9" r:id="rId4" xr:uid="{61030F94-C4B5-4BC2-8DDF-13A497F6CC87}"/>
+    <hyperlink ref="B8" r:id="rId4" xr:uid="{61030F94-C4B5-4BC2-8DDF-13A497F6CC87}"/>
     <hyperlink ref="B7" r:id="rId5" xr:uid="{7DE8905F-C6C3-47D1-8F2A-8ED5DF060050}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1065,534 +1057,534 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92A2A11A-8C34-4DB0-87EC-6C11DACD08FD}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="182.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="182.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2">
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7">
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10">
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11">
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12">
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13">
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B14">
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15">
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16">
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17">
         <v>5.5</v>
       </c>
       <c r="C17" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18">
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B19">
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B20">
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21">
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B22">
         <v>7.5</v>
       </c>
       <c r="C22" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B23">
         <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B24">
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B25">
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26">
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B27">
         <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28">
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29">
         <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30">
         <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31">
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32">
         <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B33">
         <v>8.5</v>
       </c>
       <c r="C33" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B34">
         <v>8</v>
       </c>
       <c r="C34" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B35">
         <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B36">
         <v>7</v>
       </c>
       <c r="C36" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B37">
         <v>6</v>
       </c>
       <c r="C37" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B38">
         <v>7</v>
       </c>
       <c r="C38" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B39">
         <v>9</v>
       </c>
       <c r="C39" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B40">
         <v>1.5</v>
       </c>
       <c r="C40" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B41">
         <v>7.5</v>
       </c>
       <c r="C41" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B42">
         <v>8.5</v>
       </c>
       <c r="C42" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B43">
         <v>6</v>
       </c>
       <c r="C43" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B44">
         <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B45">
         <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>